<commit_message>
re-recorded 2a and changed report part for 2a
</commit_message>
<xml_diff>
--- a/Lin_Rohner_lab4/Data_lab4A_stiction torque/data_lab4A_stiction torque_01_ccw.xlsx
+++ b/Lin_Rohner_lab4/Data_lab4A_stiction torque/data_lab4A_stiction torque_01_ccw.xlsx
@@ -76,7 +76,7 @@
         <v>-0.003550</v>
       </c>
       <c r="C2" s="1">
-        <v>10.139816</v>
+        <v>6.361236</v>
       </c>
       <c r="D2" s="1">
         <v>0.000000</v>
@@ -87,10 +87,10 @@
         <v>1.000000</v>
       </c>
       <c r="B3" s="1">
-        <v>0.000735</v>
+        <v>-0.007835</v>
       </c>
       <c r="C3" s="1">
-        <v>10.139816</v>
+        <v>6.361236</v>
       </c>
       <c r="D3" s="1">
         <v>0.000000</v>
@@ -101,10 +101,10 @@
         <v>2.000000</v>
       </c>
       <c r="B4" s="1">
-        <v>0.005020</v>
+        <v>-0.012120</v>
       </c>
       <c r="C4" s="1">
-        <v>10.139816</v>
+        <v>6.361236</v>
       </c>
       <c r="D4" s="1">
         <v>0.000000</v>
@@ -115,10 +115,10 @@
         <v>3.000000</v>
       </c>
       <c r="B5" s="1">
-        <v>0.009305</v>
+        <v>-0.016405</v>
       </c>
       <c r="C5" s="1">
-        <v>10.139816</v>
+        <v>6.361236</v>
       </c>
       <c r="D5" s="1">
         <v>0.000000</v>
@@ -129,10 +129,10 @@
         <v>4.000000</v>
       </c>
       <c r="B6" s="1">
-        <v>0.013590</v>
+        <v>-0.020690</v>
       </c>
       <c r="C6" s="1">
-        <v>10.139816</v>
+        <v>6.361236</v>
       </c>
       <c r="D6" s="1">
         <v>0.000000</v>
@@ -143,10 +143,10 @@
         <v>5.000000</v>
       </c>
       <c r="B7" s="1">
-        <v>0.017875</v>
+        <v>-0.024975</v>
       </c>
       <c r="C7" s="1">
-        <v>10.139816</v>
+        <v>6.361236</v>
       </c>
       <c r="D7" s="1">
         <v>0.000000</v>
@@ -157,13 +157,13 @@
         <v>6.000000</v>
       </c>
       <c r="B8" s="1">
-        <v>0.022160</v>
+        <v>-0.029260</v>
       </c>
       <c r="C8" s="1">
-        <v>10.090744</v>
+        <v>6.557526</v>
       </c>
       <c r="D8" s="1">
-        <v>0.049072</v>
+        <v>0.196290</v>
       </c>
     </row>
     <row r="9">
@@ -171,13 +171,13 @@
         <v>7.000000</v>
       </c>
       <c r="B9" s="1">
-        <v>0.026445</v>
+        <v>-0.033545</v>
       </c>
       <c r="C9" s="1">
-        <v>10.041671</v>
+        <v>6.655671</v>
       </c>
       <c r="D9" s="1">
-        <v>0.049072</v>
+        <v>0.294435</v>
       </c>
     </row>
     <row r="10">
@@ -185,13 +185,13 @@
         <v>8.000000</v>
       </c>
       <c r="B10" s="1">
-        <v>0.030730</v>
+        <v>-0.037830</v>
       </c>
       <c r="C10" s="1">
-        <v>9.943526</v>
+        <v>6.901033</v>
       </c>
       <c r="D10" s="1">
-        <v>0.098145</v>
+        <v>0.539797</v>
       </c>
     </row>
     <row r="11">
@@ -199,13 +199,13 @@
         <v>9.000000</v>
       </c>
       <c r="B11" s="1">
-        <v>0.035015</v>
+        <v>-0.042115</v>
       </c>
       <c r="C11" s="1">
-        <v>8.913004</v>
+        <v>7.048250</v>
       </c>
       <c r="D11" s="1">
-        <v>1.030522</v>
+        <v>0.687015</v>
       </c>
     </row>
   </sheetData>

</xml_diff>